<commit_message>
Update and flag CG82-1 profile date
</commit_message>
<xml_diff>
--- a/sources/gastaldello2024/Monte Rosa Boreholes.xlsx
+++ b/sources/gastaldello2024/Monte Rosa Boreholes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gastalde\AppData\Local\Microsoft\Windows\INetCache\Content.Outlook\53NIEHHT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\bigdata\Science\Geosciences\PhysicalGeography\GastaldelloM\Colle Gnifetti\01 Subsurface Data\Boreholes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03AF67F4-CE2D-4C29-A988-F8337BF51EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3E9C6C-D217-4C36-BC0F-6A4E989DB351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="borehole" sheetId="4" r:id="rId1"/>
@@ -2691,9 +2691,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F623E8F3-726A-447F-9519-BA025FD55A53}">
   <dimension ref="A1:S90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5708,7 +5708,7 @@
         <v>7.8769679999999997</v>
       </c>
       <c r="J53" s="64">
-        <v>4425</v>
+        <v>4452</v>
       </c>
       <c r="K53" s="64" t="s">
         <v>81</v>
@@ -7043,9 +7043,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S1055"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L21" sqref="L21"/>
+      <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>